<commit_message>
Removed border of the plots.
</commit_message>
<xml_diff>
--- a/analysis/joint_probs/joint_probs.xlsx
+++ b/analysis/joint_probs/joint_probs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhangks98/Documents/ETH/FS2021/FastCode/team11/analysis/joint_probs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C9713C-7CC9-B944-9968-E7363F239EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC487F4-C25F-9B49-8A23-C218FCAFF4F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5980" yWindow="2800" windowWidth="27240" windowHeight="16440" xr2:uid="{A2A76CFD-3413-2B49-B39A-987B25DA7D6F}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="tsne_full_100" localSheetId="0">joint_probs!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1338,6 +1338,11 @@
     <c:showDLblsOverMax val="0"/>
     <c:extLst/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
   <c:txPr>
     <a:bodyPr/>
     <a:lstStyle/>
@@ -2118,6 +2123,11 @@
     <c:showDLblsOverMax val="0"/>
     <c:extLst/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
   <c:txPr>
     <a:bodyPr/>
     <a:lstStyle/>
@@ -2628,8 +2638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77CC58FE-9F23-3841-960A-E23A034116BE}">
   <dimension ref="A1:P64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2704,7 +2714,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4">
-        <f>2^A3</f>
+        <f t="shared" ref="B3:B13" si="0">2^A3</f>
         <v>4</v>
       </c>
       <c r="C3">
@@ -2715,6 +2725,10 @@
       </c>
       <c r="E3">
         <v>38213.599999999999</v>
+      </c>
+      <c r="F3" s="1">
+        <f>C3/E3</f>
+        <v>1.2051625599263089</v>
       </c>
       <c r="I3" s="1">
         <f>2329*B3^2 -728*B3</f>
@@ -2750,7 +2764,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4">
-        <f>2^A4</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="C4">
@@ -2762,28 +2776,32 @@
       <c r="E4">
         <v>111080</v>
       </c>
+      <c r="F4" s="1">
+        <f t="shared" ref="F4:F13" si="1">C4/E4</f>
+        <v>1.6347947425279079</v>
+      </c>
       <c r="I4" s="1">
-        <f t="shared" ref="I4:I13" si="0">2329*B4^2 -728*B4</f>
+        <f t="shared" ref="I4:I13" si="2">2329*B4^2 -728*B4</f>
         <v>143232</v>
       </c>
       <c r="J4" s="1">
-        <f t="shared" ref="J4:J13" si="1">1938.5*B4^2 + 1230.5*B4</f>
+        <f t="shared" ref="J4:J13" si="3">1938.5*B4^2 + 1230.5*B4</f>
         <v>133908</v>
       </c>
       <c r="K4" s="1">
-        <f t="shared" ref="K4:K13" si="2">2788.5*B4^2 + 380.5*B4</f>
+        <f t="shared" ref="K4:K13" si="4">2788.5*B4^2 + 380.5*B4</f>
         <v>181508</v>
       </c>
       <c r="L4" s="1">
-        <f t="shared" ref="L4:L13" si="3">I4/C4</f>
+        <f t="shared" ref="L4:L13" si="5">I4/C4</f>
         <v>0.78875287043002762</v>
       </c>
       <c r="M4" s="1">
-        <f t="shared" ref="M4:M13" si="4">J4/D4</f>
+        <f t="shared" ref="M4:M13" si="6">J4/D4</f>
         <v>1.0344380069524912</v>
       </c>
       <c r="N4" s="1">
-        <f t="shared" ref="N4:N13" si="5">K4/E4</f>
+        <f t="shared" ref="N4:N13" si="7">K4/E4</f>
         <v>1.6340295282679149</v>
       </c>
       <c r="O4" s="1"/>
@@ -2793,7 +2811,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4">
-        <f>2^A5</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="C5">
@@ -2805,28 +2823,32 @@
       <c r="E5">
         <v>190216</v>
       </c>
+      <c r="F5" s="1">
+        <f t="shared" si="1"/>
+        <v>3.9141081717626278</v>
+      </c>
       <c r="I5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>584576</v>
       </c>
       <c r="J5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>515944</v>
       </c>
       <c r="K5" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>719944</v>
       </c>
       <c r="L5" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.78516532666421324</v>
       </c>
       <c r="M5" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.0837998449745931</v>
       </c>
       <c r="N5" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.7848761408083442</v>
       </c>
       <c r="O5" s="1"/>
@@ -2836,7 +2858,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4">
-        <f>2^A6</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="C6" s="1">
@@ -2848,28 +2870,32 @@
       <c r="E6">
         <v>641103</v>
       </c>
+      <c r="F6" s="1">
+        <f t="shared" si="1"/>
+        <v>4.7955788695420241</v>
+      </c>
       <c r="I6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2361600</v>
       </c>
       <c r="J6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2024400</v>
       </c>
       <c r="K6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2867600</v>
       </c>
       <c r="L6" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.7681348919810308</v>
       </c>
       <c r="M6" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.0581944204864433</v>
       </c>
       <c r="N6" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4.472916208471962</v>
       </c>
       <c r="O6" s="1"/>
@@ -2879,7 +2905,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4">
-        <f>2^A7</f>
+        <f t="shared" si="0"/>
         <v>64</v>
       </c>
       <c r="C7" s="1">
@@ -2891,28 +2917,32 @@
       <c r="E7" s="1">
         <v>2106200</v>
       </c>
+      <c r="F7" s="1">
+        <f t="shared" si="1"/>
+        <v>5.8888044820055079</v>
+      </c>
       <c r="I7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9492992</v>
       </c>
       <c r="J7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8018848</v>
       </c>
       <c r="K7" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>11446048</v>
       </c>
       <c r="L7" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.76537869870192698</v>
       </c>
       <c r="M7" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.0970956990953817</v>
       </c>
       <c r="N7" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5.4344544677618458</v>
       </c>
       <c r="O7" s="1"/>
@@ -2922,7 +2952,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="4">
-        <f>2^A8</f>
+        <f t="shared" si="0"/>
         <v>128</v>
       </c>
       <c r="C8" s="1">
@@ -2934,28 +2964,32 @@
       <c r="E8" s="1">
         <v>7488260</v>
       </c>
+      <c r="F8" s="1">
+        <f t="shared" si="1"/>
+        <v>6.7318976638097503</v>
+      </c>
       <c r="I8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>38065152</v>
       </c>
       <c r="J8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>31917888</v>
       </c>
       <c r="K8" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>45735488</v>
       </c>
       <c r="L8" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.75510813287786993</v>
       </c>
       <c r="M8" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.1124471273822303</v>
       </c>
       <c r="N8" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>6.107625536506478</v>
       </c>
       <c r="O8" s="1"/>
@@ -2965,7 +2999,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="4">
-        <f>2^A9</f>
+        <f t="shared" si="0"/>
         <v>256</v>
       </c>
       <c r="C9" s="1">
@@ -2977,28 +3011,32 @@
       <c r="E9" s="1">
         <v>28692100</v>
       </c>
+      <c r="F9" s="1">
+        <f t="shared" si="1"/>
+        <v>7.0179945002282862</v>
+      </c>
       <c r="I9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>152446976</v>
       </c>
       <c r="J9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>127356544</v>
       </c>
       <c r="K9" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>182844544</v>
       </c>
       <c r="L9" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.75708293065687993</v>
       </c>
       <c r="M9" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.1142499781273514</v>
       </c>
       <c r="N9" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>6.3726441773171016</v>
       </c>
       <c r="O9" s="1"/>
@@ -3008,7 +3046,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="4">
-        <f>2^A10</f>
+        <f t="shared" si="0"/>
         <v>512</v>
       </c>
       <c r="C10" s="1">
@@ -3020,28 +3058,32 @@
       <c r="E10" s="1">
         <v>114756000</v>
       </c>
+      <c r="F10" s="1">
+        <f t="shared" si="1"/>
+        <v>7.0733817839590083</v>
+      </c>
       <c r="I10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>610160640</v>
       </c>
       <c r="J10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>508796160</v>
       </c>
       <c r="K10" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>731183360</v>
       </c>
       <c r="L10" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.75169504492351358</v>
       </c>
       <c r="M10" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.0979632283124729</v>
       </c>
       <c r="N10" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>6.3716351214751299</v>
       </c>
       <c r="O10" s="1"/>
@@ -3051,7 +3093,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="4">
-        <f>2^A11</f>
+        <f t="shared" si="0"/>
         <v>1024</v>
       </c>
       <c r="C11" s="1">
@@ -3063,28 +3105,32 @@
       <c r="E11" s="1">
         <v>469240000</v>
       </c>
+      <c r="F11" s="1">
+        <f t="shared" si="1"/>
+        <v>7.0664478731565934</v>
+      </c>
       <c r="I11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2441388032</v>
       </c>
       <c r="J11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2033924608</v>
       </c>
       <c r="K11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2924343808</v>
       </c>
       <c r="L11" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.73627596822543773</v>
       </c>
       <c r="M11" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.0449083785852629</v>
       </c>
       <c r="N11" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>6.2320855170062233</v>
       </c>
       <c r="O11" s="1"/>
@@ -3094,7 +3140,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="4">
-        <f>2^A12</f>
+        <f t="shared" si="0"/>
         <v>2048</v>
       </c>
       <c r="C12" s="1">
@@ -3106,28 +3152,32 @@
       <c r="E12" s="1">
         <v>1952260000</v>
       </c>
+      <c r="F12" s="1">
+        <f t="shared" si="1"/>
+        <v>6.8540563244649793</v>
+      </c>
       <c r="I12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9767043072</v>
       </c>
       <c r="J12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8133178368</v>
       </c>
       <c r="K12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>11696595968</v>
       </c>
       <c r="L12" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.72992422572472704</v>
       </c>
       <c r="M12" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.01964888741232</v>
       </c>
       <c r="N12" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5.9913105672400189</v>
       </c>
       <c r="O12" s="1"/>
@@ -3137,7 +3187,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="4">
-        <f>2^A13</f>
+        <f t="shared" si="0"/>
         <v>4096</v>
       </c>
       <c r="C13" s="1">
@@ -3149,28 +3199,32 @@
       <c r="E13" s="1">
         <v>7994530000</v>
       </c>
+      <c r="F13" s="1">
+        <f t="shared" si="1"/>
+        <v>6.7067482391084905</v>
+      </c>
       <c r="I13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>39071154176</v>
       </c>
       <c r="J13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>32527673344</v>
       </c>
       <c r="K13" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>46784825344</v>
       </c>
       <c r="L13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.72870424612951412</v>
       </c>
       <c r="M13" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.0123139967633512</v>
       </c>
       <c r="N13" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5.8521045444822901</v>
       </c>
       <c r="O13" s="1"/>

</xml_diff>